<commit_message>
Add race class and model interface capture completed round_count
</commit_message>
<xml_diff>
--- a/test/core_test/stf2.xlsx
+++ b/test/core_test/stf2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Environment-Framework\test\core_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5B85C3-BBDF-4817-9072-F2146A74F2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA64A95-914F-4E13-83EB-412CE2734253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{19C3DDC4-AFB1-4D82-AE89-12F56748A908}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL19" sqref="AL19"/>
+      <selection activeCell="AM25" sqref="AM25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,119 +484,119 @@
         <v>0</v>
       </c>
       <c r="C1" s="1">
-        <f>B1+1</f>
+        <f t="shared" ref="C1:AE1" si="0">B1+1</f>
         <v>1</v>
       </c>
       <c r="D1" s="1">
-        <f>C1+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E1" s="1">
-        <f>D1+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F1" s="1">
-        <f>E1+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G1" s="1">
-        <f>F1+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H1" s="1">
-        <f>G1+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I1" s="1">
-        <f>H1+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="J1" s="1">
-        <f>I1+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="K1" s="1">
-        <f>J1+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L1" s="1">
-        <f>K1+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="M1" s="1">
-        <f>L1+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="N1" s="1">
-        <f>M1+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="O1" s="1">
-        <f>N1+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="P1" s="1">
-        <f>O1+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="Q1" s="1">
-        <f>P1+1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="R1" s="1">
-        <f>Q1+1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="S1" s="1">
-        <f>R1+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="T1" s="1">
-        <f>S1+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="U1" s="1">
-        <f>T1+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="V1" s="1">
-        <f>U1+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="W1" s="1">
-        <f>V1+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="X1" s="1">
-        <f>W1+1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="Y1" s="1">
-        <f>X1+1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="Z1" s="1">
-        <f>Y1+1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="AA1" s="1">
-        <f>Z1+1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="AB1" s="1">
-        <f>AA1+1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="AC1" s="1">
-        <f>AB1+1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="AD1" s="1">
-        <f>AC1+1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="AE1" s="1">
-        <f>AD1+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
@@ -637,7 +637,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A21" si="1">A2+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="2"/>
@@ -675,7 +675,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <f>A3+1</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
@@ -713,7 +713,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <f>A4+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B5" s="2"/>
@@ -730,9 +730,9 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
@@ -751,7 +751,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <f>A5+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B6" s="2"/>
@@ -789,7 +789,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <f>A6+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B7" s="2"/>
@@ -833,7 +833,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <f>A7+1</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
@@ -873,7 +873,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <f>A8+1</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B9" s="2"/>
@@ -890,9 +890,9 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -913,7 +913,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <f>A9+1</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B10" s="2"/>
@@ -953,7 +953,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <f>A10+1</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B11" s="2"/>
@@ -993,7 +993,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <f>A11+1</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B12" s="2"/>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <f>A12+1</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B13" s="2"/>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <f>A13+1</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B14" s="2"/>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <f>A14+1</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B15" s="2"/>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <f>A15+1</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B16" s="2"/>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <f>A16+1</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B17" s="2"/>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <f>A17+1</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B18" s="2"/>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <f>A18+1</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B19" s="2"/>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <f>A19+1</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B20" s="2"/>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <f>A20+1</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B21" s="2"/>

</xml_diff>